<commit_message>
Updated to include other categories.
</commit_message>
<xml_diff>
--- a/Random/HBR/Podcast.xlsx
+++ b/Random/HBR/Podcast.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nssf-my.sharepoint.com/personal/amakubuya_nssfug_org/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmuwanga\Developer\Learning-PyDS\Random\HBR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0A20FB3-96F7-47C5-B76E-EBDED77BB59F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="innovation" sheetId="1" r:id="rId1"/>
     <sheet name="Leadership" sheetId="3" r:id="rId2"/>
     <sheet name="Personal Dev't" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -178,9 +179,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -217,16 +218,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -508,26 +509,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -535,15 +536,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>660</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>659</v>
       </c>
@@ -551,7 +552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>651</v>
       </c>
@@ -559,7 +560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>648</v>
       </c>
@@ -567,7 +568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>647</v>
       </c>
@@ -575,7 +576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>642</v>
       </c>
@@ -583,15 +584,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>640</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>630</v>
       </c>
@@ -599,7 +600,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>628</v>
       </c>
@@ -607,7 +608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>625</v>
       </c>
@@ -615,7 +616,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>616</v>
       </c>
@@ -632,25 +633,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="2" max="2" width="64.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -658,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>654</v>
       </c>
@@ -666,7 +667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>653</v>
       </c>
@@ -674,7 +675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>652</v>
       </c>
@@ -682,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>650</v>
       </c>
@@ -690,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>649</v>
       </c>
@@ -698,7 +699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>645</v>
       </c>
@@ -706,7 +707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>644</v>
       </c>
@@ -714,7 +715,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>639</v>
       </c>
@@ -722,7 +723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>638</v>
       </c>
@@ -730,7 +731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>637</v>
       </c>
@@ -738,7 +739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>629</v>
       </c>
@@ -746,7 +747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>627</v>
       </c>
@@ -754,7 +755,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>626</v>
       </c>
@@ -762,7 +763,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>623</v>
       </c>
@@ -770,7 +771,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>622</v>
       </c>
@@ -778,7 +779,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>621</v>
       </c>
@@ -786,7 +787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>620</v>
       </c>
@@ -794,7 +795,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>617</v>
       </c>
@@ -802,7 +803,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>615</v>
       </c>
@@ -810,7 +811,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>612</v>
       </c>
@@ -818,7 +819,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>611</v>
       </c>
@@ -826,7 +827,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>610</v>
       </c>
@@ -843,26 +844,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="57.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -870,7 +871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>658</v>
       </c>
@@ -878,7 +879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>657</v>
       </c>
@@ -886,7 +887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>646</v>
       </c>
@@ -894,7 +895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>634</v>
       </c>
@@ -902,7 +903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>633</v>
       </c>
@@ -910,7 +911,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>631</v>
       </c>
@@ -918,7 +919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>624</v>
       </c>
@@ -926,7 +927,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>619</v>
       </c>
@@ -934,7 +935,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>614</v>
       </c>
@@ -942,7 +943,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>613</v>
       </c>
@@ -950,7 +951,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>608</v>
       </c>

</xml_diff>